<commit_message>
new simpler methods script runs
</commit_message>
<xml_diff>
--- a/data/scenario_key.xlsx
+++ b/data/scenario_key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Documents/GitHub/africa_export/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0311C21B-7056-8148-8AA4-F56BFAD90811}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9969FFC0-3CCB-7247-B241-D5975AEB4FE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{A096658D-A36F-DE43-9E12-AEAA48E6A1BD}"/>
   </bookViews>
@@ -74,9 +74,6 @@
     <t>by_city</t>
   </si>
   <si>
-    <t>by_population</t>
-  </si>
-  <si>
     <t>Shorter prevalence</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>M&amp;B ascertainment rate</t>
+  </si>
+  <si>
+    <t>by_pop</t>
   </si>
 </sst>
 </file>
@@ -464,7 +464,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -544,7 +544,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <f>$D$2</f>
@@ -565,7 +565,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5">
         <f t="shared" ref="D5:D10" si="0">$D$2</f>
@@ -586,7 +586,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
@@ -607,7 +607,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <f>SUM($D$2/10)</f>
@@ -628,7 +628,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8">
         <f>SUM($D$2*10)</f>
@@ -649,7 +649,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
@@ -670,7 +670,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
@@ -680,7 +680,7 @@
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -691,7 +691,7 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11">
         <v>2</v>
@@ -711,7 +711,7 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12">
         <v>1.4</v>

</xml_diff>

<commit_message>
Merged clean repo with private working repo
</commit_message>
<xml_diff>
--- a/data/scenario_key.xlsx
+++ b/data/scenario_key.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Documents/GitHub/africa_export/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/Documents/export_paper_tmp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9969FFC0-3CCB-7247-B241-D5975AEB4FE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C86848-F6C1-0B47-B3AE-8D032853E1D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{A096658D-A36F-DE43-9E12-AEAA48E6A1BD}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>scenario_id</t>
   </si>
@@ -53,9 +53,6 @@
     <t>main</t>
   </si>
   <si>
-    <t>optional</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -93,12 +90,6 @@
   </si>
   <si>
     <t>Assign province cases to city proportional to population</t>
-  </si>
-  <si>
-    <t>Verity ascertainment rate</t>
-  </si>
-  <si>
-    <t>M&amp;B ascertainment rate</t>
   </si>
   <si>
     <t>by_pop</t>
@@ -461,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{743793E0-923D-804F-9D1D-E0D5649A6992}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A11" sqref="A11:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -484,7 +475,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -504,7 +495,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2">
         <v>5.1440000000000001</v>
@@ -513,7 +504,7 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -524,16 +515,16 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
         <v>10</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -544,7 +535,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4">
         <f>$D$2</f>
@@ -554,7 +545,7 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -565,7 +556,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5">
         <f t="shared" ref="D5:D10" si="0">$D$2</f>
@@ -575,7 +566,7 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -586,17 +577,17 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
         <v>5.1440000000000001</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
         <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -607,7 +598,7 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7">
         <f>SUM($D$2/10)</f>
@@ -617,7 +608,7 @@
         <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -628,7 +619,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8">
         <f>SUM($D$2*10)</f>
@@ -638,7 +629,7 @@
         <v>5</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -649,7 +640,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
@@ -659,7 +650,7 @@
         <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -670,7 +661,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
@@ -680,47 +671,7 @@
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11">
-        <v>5</v>
-      </c>
-      <c r="F11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12">
-        <v>1.4</v>
-      </c>
-      <c r="E12">
-        <v>5</v>
-      </c>
-      <c r="F12" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>